<commit_message>
Updated Brackets, Box Scores
Data Input to EOD 4/22/25
</commit_message>
<xml_diff>
--- a/2024_2025/Playoffs/BoxScores.xlsx
+++ b/2024_2025/Playoffs/BoxScores.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024_2025\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024_2025\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C0ED10-E6CC-4993-A85B-D3C1E506BC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -32,11 +31,11 @@
     <sheet name="Offense (4-21-25)" sheetId="17" r:id="rId17"/>
     <sheet name="Goalies (4-21-25)" sheetId="18" r:id="rId18"/>
     <sheet name="Offense (4-22-25)" sheetId="19" r:id="rId19"/>
-    <sheet name="Rosters (Offense - 24)" sheetId="10" r:id="rId20"/>
-    <sheet name="Goalies (4-22-25)" sheetId="20" r:id="rId21"/>
-    <sheet name="Rosters (Goalies - 3)" sheetId="11" r:id="rId22"/>
-    <sheet name="Offense (4-23-25)" sheetId="22" r:id="rId23"/>
-    <sheet name="Goalies (4-23-25)" sheetId="23" r:id="rId24"/>
+    <sheet name="Goalies (4-22-25)" sheetId="20" r:id="rId20"/>
+    <sheet name="Offense (4-23-25)" sheetId="22" r:id="rId21"/>
+    <sheet name="Rosters (Offense - 24)" sheetId="10" r:id="rId22"/>
+    <sheet name="Goalies (4-23-25)" sheetId="23" r:id="rId23"/>
+    <sheet name="Rosters (Goalies - 3)" sheetId="11" r:id="rId24"/>
     <sheet name="Offense (4-24-25)" sheetId="25" r:id="rId25"/>
     <sheet name="Goalies (4-24-25)" sheetId="26" r:id="rId26"/>
     <sheet name="Offense (4-25-25)" sheetId="28" r:id="rId27"/>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2900" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="531">
   <si>
     <t>Carolina Hurricanes</t>
   </si>
@@ -1654,7 +1653,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -2215,7 +2214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2493,17 +2492,17 @@
     <mergeCell ref="A43:B43"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" location="'Scores (4-19-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" location="'Scores (4-20-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" location="'Scores (4-21-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" location="'Scores (4-22-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6:B10" location="'Scores (4-22-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B6" location="'Scores (4-23-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B7" location="'Scores (4-24-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" location="'Scores (4-25-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B9" location="'Scores (4-26-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" location="'Scores (4-27-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" location="'Scores (4-28-25)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B2" location="'Scores (4-19-25)'!A1" display="Scores"/>
+    <hyperlink ref="B3" location="'Scores (4-20-25)'!A1" display="Scores"/>
+    <hyperlink ref="B4" location="'Scores (4-21-25)'!A1" display="Scores"/>
+    <hyperlink ref="B5" location="'Scores (4-22-25)'!A1" display="Scores"/>
+    <hyperlink ref="B6:B10" location="'Scores (4-22-25)'!A1" display="Scores"/>
+    <hyperlink ref="B6" location="'Scores (4-23-25)'!A1" display="Scores"/>
+    <hyperlink ref="B7" location="'Scores (4-24-25)'!A1" display="Scores"/>
+    <hyperlink ref="B8" location="'Scores (4-25-25)'!A1" display="Scores"/>
+    <hyperlink ref="B9" location="'Scores (4-26-25)'!A1" display="Scores"/>
+    <hyperlink ref="B10" location="'Scores (4-27-25)'!A1" display="Scores"/>
+    <hyperlink ref="B11" location="'Scores (4-28-25)'!A1" display="Scores"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2511,7 +2510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2613,21 +2612,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="A7" location="'Offense (4-26-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="A8" location="'Goalies (4-26-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A7" location="'Offense (4-26-25)'!A1" display="Offense"/>
+    <hyperlink ref="A8" location="'Goalies (4-26-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2640,7 +2639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2742,21 +2741,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="A7" location="'Offense (4-27-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="A8" location="'Goalies (4-27-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A7" location="'Offense (4-27-25)'!A1" display="Offense"/>
+    <hyperlink ref="A8" location="'Goalies (4-27-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2769,7 +2768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2855,21 +2854,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="A7" location="'Offense (4-27-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
-    <hyperlink ref="A8" location="'Goalies (4-27-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A7" location="'Offense (4-27-25)'!A1" display="Offense"/>
+    <hyperlink ref="A8" location="'Goalies (4-27-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2882,7 +2881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U94"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7478,11 +7477,11 @@
     <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:T55">
+  <sortState ref="A38:T55">
     <sortCondition ref="A38:A55"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-19-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-19-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7490,7 +7489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7706,7 +7705,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-19-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-19-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7714,7 +7713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U130"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14526,11 +14525,11 @@
     <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A75:T92">
+  <sortState ref="A75:T92">
     <sortCondition ref="A75"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-20-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-20-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14538,7 +14537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14822,7 +14821,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-20-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-20-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -14830,7 +14829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U166"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -23922,11 +23921,11 @@
     <row r="165" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="166" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A75:T92">
+  <sortState ref="A75:T92">
     <sortCondition ref="A75"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-21-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-21-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -23934,7 +23933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24296,7 +24295,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-21-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-21-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -24304,12 +24303,10 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:U286"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U248"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="U110" sqref="U110"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31085,256 +31082,2308 @@
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D110" s="1">
+        <v>0</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0</v>
+      </c>
+      <c r="F110" s="1">
+        <v>3</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0</v>
+      </c>
+      <c r="H110" s="1">
+        <v>1</v>
+      </c>
+      <c r="I110" s="1">
+        <v>3</v>
+      </c>
+      <c r="J110" s="1">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1">
+        <v>0</v>
+      </c>
+      <c r="L110" s="1">
+        <v>0</v>
+      </c>
+      <c r="M110" s="1">
+        <v>0</v>
+      </c>
+      <c r="N110" s="1">
+        <v>4</v>
+      </c>
+      <c r="O110" s="1">
+        <v>29</v>
+      </c>
+      <c r="P110" s="13">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="Q110" s="13">
+        <v>0</v>
+      </c>
+      <c r="R110" s="14">
+        <v>1.086111111111111</v>
+      </c>
+      <c r="S110" s="1">
+        <v>0</v>
+      </c>
+      <c r="T110" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P111" s="1"/>
-      <c r="Q111" s="1"/>
-      <c r="R111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0</v>
+      </c>
+      <c r="F111" s="1">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0</v>
+      </c>
+      <c r="H111" s="1">
+        <v>2</v>
+      </c>
+      <c r="I111" s="1">
+        <v>1</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0</v>
+      </c>
+      <c r="K111" s="1">
+        <v>0</v>
+      </c>
+      <c r="L111" s="1">
+        <v>2</v>
+      </c>
+      <c r="M111" s="1">
+        <v>2</v>
+      </c>
+      <c r="N111" s="1">
+        <v>0</v>
+      </c>
+      <c r="O111" s="1">
+        <v>20</v>
+      </c>
+      <c r="P111" s="13">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q111" s="13">
+        <v>0</v>
+      </c>
+      <c r="R111" s="13">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="S111" s="1">
+        <v>3</v>
+      </c>
+      <c r="T111" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
-      <c r="R112" s="1"/>
-    </row>
-    <row r="113" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P113" s="1"/>
-      <c r="Q113" s="1"/>
-      <c r="R113" s="1"/>
-    </row>
-    <row r="114" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
-      <c r="R114" s="1"/>
-    </row>
-    <row r="115" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P115" s="1"/>
-      <c r="Q115" s="1"/>
-      <c r="R115" s="1"/>
-    </row>
-    <row r="116" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P116" s="1"/>
-      <c r="Q116" s="1"/>
-      <c r="R116" s="1"/>
-    </row>
-    <row r="117" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P117" s="1"/>
-      <c r="Q117" s="1"/>
-      <c r="R117" s="1"/>
-    </row>
-    <row r="118" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P118" s="1"/>
-      <c r="Q118" s="1"/>
-      <c r="R118" s="1"/>
-    </row>
-    <row r="119" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P119" s="1"/>
-      <c r="Q119" s="1"/>
-      <c r="R119" s="1"/>
-    </row>
-    <row r="120" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P120" s="1"/>
-      <c r="Q120" s="1"/>
-      <c r="R120" s="1"/>
-    </row>
-    <row r="121" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P121" s="1"/>
-      <c r="Q121" s="1"/>
-      <c r="R121" s="1"/>
-    </row>
-    <row r="122" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P122" s="1"/>
-      <c r="Q122" s="1"/>
-      <c r="R122" s="1"/>
-    </row>
-    <row r="123" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P123" s="1"/>
-      <c r="Q123" s="1"/>
-      <c r="R123" s="1"/>
-    </row>
-    <row r="124" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P124" s="1"/>
-      <c r="Q124" s="1"/>
-      <c r="R124" s="1"/>
-    </row>
-    <row r="125" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P125" s="1"/>
-      <c r="Q125" s="1"/>
-      <c r="R125" s="1"/>
-    </row>
-    <row r="126" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P126" s="1"/>
-      <c r="Q126" s="1"/>
-      <c r="R126" s="1"/>
-    </row>
-    <row r="127" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P127" s="1"/>
-      <c r="Q127" s="1"/>
-      <c r="R127" s="1"/>
-    </row>
-    <row r="128" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P128" s="1"/>
-      <c r="Q128" s="1"/>
-      <c r="R128" s="1"/>
-    </row>
-    <row r="129" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P129" s="1"/>
-      <c r="Q129" s="1"/>
-      <c r="R129" s="1"/>
-    </row>
-    <row r="130" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P130" s="1"/>
-      <c r="Q130" s="1"/>
-      <c r="R130" s="1"/>
-    </row>
-    <row r="131" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P131" s="1"/>
-      <c r="Q131" s="1"/>
-      <c r="R131" s="1"/>
-    </row>
-    <row r="132" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P132" s="1"/>
-      <c r="Q132" s="1"/>
-      <c r="R132" s="1"/>
-    </row>
-    <row r="133" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P133" s="1"/>
-      <c r="Q133" s="1"/>
-      <c r="R133" s="1"/>
-    </row>
-    <row r="134" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P134" s="1"/>
-      <c r="Q134" s="1"/>
-      <c r="R134" s="1"/>
-    </row>
-    <row r="135" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P135" s="1"/>
-      <c r="Q135" s="1"/>
-      <c r="R135" s="1"/>
-    </row>
-    <row r="136" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P136" s="1"/>
-      <c r="Q136" s="1"/>
-      <c r="R136" s="1"/>
-    </row>
-    <row r="137" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P137" s="1"/>
-      <c r="Q137" s="1"/>
-      <c r="R137" s="1"/>
-    </row>
-    <row r="138" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P138" s="1"/>
-      <c r="Q138" s="1"/>
-      <c r="R138" s="1"/>
-    </row>
-    <row r="139" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P139" s="1"/>
-      <c r="Q139" s="1"/>
-      <c r="R139" s="1"/>
-    </row>
-    <row r="140" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P140" s="1"/>
-      <c r="Q140" s="1"/>
-      <c r="R140" s="1"/>
-    </row>
-    <row r="141" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P141" s="1"/>
-      <c r="Q141" s="1"/>
-      <c r="R141" s="1"/>
-    </row>
-    <row r="142" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P142" s="1"/>
-      <c r="Q142" s="1"/>
-      <c r="R142" s="1"/>
-    </row>
-    <row r="143" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P143" s="1"/>
-      <c r="Q143" s="1"/>
-      <c r="R143" s="1"/>
-    </row>
-    <row r="144" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P144" s="1"/>
-      <c r="Q144" s="1"/>
-      <c r="R144" s="1"/>
-    </row>
-    <row r="145" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P145" s="1"/>
-      <c r="Q145" s="1"/>
-      <c r="R145" s="1"/>
-    </row>
-    <row r="146" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0</v>
+      </c>
+      <c r="G112" s="1">
+        <v>0</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0</v>
+      </c>
+      <c r="I112" s="1">
+        <v>1</v>
+      </c>
+      <c r="J112" s="1">
+        <v>0</v>
+      </c>
+      <c r="K112" s="1">
+        <v>0</v>
+      </c>
+      <c r="L112" s="1">
+        <v>0</v>
+      </c>
+      <c r="M112" s="1">
+        <v>0</v>
+      </c>
+      <c r="N112" s="1">
+        <v>1</v>
+      </c>
+      <c r="O112" s="1">
+        <v>22</v>
+      </c>
+      <c r="P112" s="13">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="Q112" s="13">
+        <v>0</v>
+      </c>
+      <c r="R112" s="13">
+        <v>0.65625</v>
+      </c>
+      <c r="S112" s="1">
+        <v>0</v>
+      </c>
+      <c r="T112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0</v>
+      </c>
+      <c r="F113" s="1">
+        <v>2</v>
+      </c>
+      <c r="G113" s="1">
+        <v>0</v>
+      </c>
+      <c r="H113" s="1">
+        <v>2</v>
+      </c>
+      <c r="I113" s="1">
+        <v>2</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0</v>
+      </c>
+      <c r="K113" s="1">
+        <v>0</v>
+      </c>
+      <c r="L113" s="1">
+        <v>1</v>
+      </c>
+      <c r="M113" s="1">
+        <v>0</v>
+      </c>
+      <c r="N113" s="1">
+        <v>1</v>
+      </c>
+      <c r="O113" s="1">
+        <v>25</v>
+      </c>
+      <c r="P113" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q113" s="13">
+        <v>0</v>
+      </c>
+      <c r="R113" s="13">
+        <v>0.84513888888888899</v>
+      </c>
+      <c r="S113" s="1">
+        <v>0</v>
+      </c>
+      <c r="T113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D114" s="1">
+        <v>0</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0</v>
+      </c>
+      <c r="F114" s="1">
+        <v>3</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1">
+        <v>2</v>
+      </c>
+      <c r="J114" s="1">
+        <v>0</v>
+      </c>
+      <c r="K114" s="1">
+        <v>0</v>
+      </c>
+      <c r="L114" s="1">
+        <v>1</v>
+      </c>
+      <c r="M114" s="1">
+        <v>0</v>
+      </c>
+      <c r="N114" s="1">
+        <v>0</v>
+      </c>
+      <c r="O114" s="1">
+        <v>26</v>
+      </c>
+      <c r="P114" s="13">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="Q114" s="13">
+        <v>0</v>
+      </c>
+      <c r="R114" s="13">
+        <v>0.87430555555555556</v>
+      </c>
+      <c r="S114" s="1">
+        <v>0</v>
+      </c>
+      <c r="T114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0</v>
+      </c>
+      <c r="F115" s="1">
+        <v>3</v>
+      </c>
+      <c r="G115" s="1">
+        <v>3</v>
+      </c>
+      <c r="H115" s="1">
+        <v>2</v>
+      </c>
+      <c r="I115" s="1">
+        <v>3</v>
+      </c>
+      <c r="J115" s="1">
+        <v>0</v>
+      </c>
+      <c r="K115" s="1">
+        <v>0</v>
+      </c>
+      <c r="L115" s="1">
+        <v>3</v>
+      </c>
+      <c r="M115" s="1">
+        <v>0</v>
+      </c>
+      <c r="N115" s="1">
+        <v>0</v>
+      </c>
+      <c r="O115" s="1">
+        <v>24</v>
+      </c>
+      <c r="P115" s="13">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="Q115" s="13">
+        <v>0</v>
+      </c>
+      <c r="R115" s="13">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="S115" s="1">
+        <v>7</v>
+      </c>
+      <c r="T115" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1</v>
+      </c>
+      <c r="F116" s="1">
+        <v>2</v>
+      </c>
+      <c r="G116" s="1">
+        <v>0</v>
+      </c>
+      <c r="H116" s="1">
+        <v>3</v>
+      </c>
+      <c r="I116" s="1">
+        <v>1</v>
+      </c>
+      <c r="J116" s="1">
+        <v>0</v>
+      </c>
+      <c r="K116" s="1">
+        <v>0</v>
+      </c>
+      <c r="L116" s="1">
+        <v>1</v>
+      </c>
+      <c r="M116" s="1">
+        <v>1</v>
+      </c>
+      <c r="N116" s="1">
+        <v>1</v>
+      </c>
+      <c r="O116" s="1">
+        <v>29</v>
+      </c>
+      <c r="P116" s="13">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="Q116" s="13">
+        <v>0</v>
+      </c>
+      <c r="R116" s="14">
+        <v>1.04375</v>
+      </c>
+      <c r="S116" s="1">
+        <v>0</v>
+      </c>
+      <c r="T116" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D117" s="1">
+        <v>0</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1">
+        <v>0</v>
+      </c>
+      <c r="G117" s="1">
+        <v>1</v>
+      </c>
+      <c r="H117" s="1">
+        <v>0</v>
+      </c>
+      <c r="I117" s="1">
+        <v>2</v>
+      </c>
+      <c r="J117" s="1">
+        <v>0</v>
+      </c>
+      <c r="K117" s="1">
+        <v>0</v>
+      </c>
+      <c r="L117" s="1">
+        <v>2</v>
+      </c>
+      <c r="M117" s="1">
+        <v>0</v>
+      </c>
+      <c r="N117" s="1">
+        <v>0</v>
+      </c>
+      <c r="O117" s="1">
+        <v>10</v>
+      </c>
+      <c r="P117" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q117" s="13">
+        <v>0</v>
+      </c>
+      <c r="R117" s="13">
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="S117" s="1">
+        <v>0</v>
+      </c>
+      <c r="T117" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D118" s="1">
+        <v>2</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+      <c r="F118" s="1">
+        <v>2</v>
+      </c>
+      <c r="G118" s="1">
+        <v>4</v>
+      </c>
+      <c r="H118" s="1">
+        <v>1</v>
+      </c>
+      <c r="I118" s="1">
+        <v>4</v>
+      </c>
+      <c r="J118" s="1">
+        <v>0</v>
+      </c>
+      <c r="K118" s="1">
+        <v>0</v>
+      </c>
+      <c r="L118" s="1">
+        <v>2</v>
+      </c>
+      <c r="M118" s="1">
+        <v>0</v>
+      </c>
+      <c r="N118" s="1">
+        <v>1</v>
+      </c>
+      <c r="O118" s="1">
+        <v>23</v>
+      </c>
+      <c r="P118" s="13">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="Q118" s="13">
+        <v>0</v>
+      </c>
+      <c r="R118" s="13">
+        <v>0.78194444444444444</v>
+      </c>
+      <c r="S118" s="1">
+        <v>0</v>
+      </c>
+      <c r="T118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D119" s="1">
+        <v>0</v>
+      </c>
+      <c r="E119" s="1">
+        <v>0</v>
+      </c>
+      <c r="F119" s="1">
+        <v>0</v>
+      </c>
+      <c r="G119" s="1">
+        <v>0</v>
+      </c>
+      <c r="H119" s="1">
+        <v>0</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0</v>
+      </c>
+      <c r="J119" s="1">
+        <v>0</v>
+      </c>
+      <c r="K119" s="1">
+        <v>0</v>
+      </c>
+      <c r="L119" s="1">
+        <v>0</v>
+      </c>
+      <c r="M119" s="1">
+        <v>0</v>
+      </c>
+      <c r="N119" s="1">
+        <v>0</v>
+      </c>
+      <c r="O119" s="1">
+        <v>11</v>
+      </c>
+      <c r="P119" s="13">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="Q119" s="13">
+        <v>0</v>
+      </c>
+      <c r="R119" s="13">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="S119" s="1">
+        <v>2</v>
+      </c>
+      <c r="T119" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1">
+        <v>2</v>
+      </c>
+      <c r="H120" s="1">
+        <v>0</v>
+      </c>
+      <c r="I120" s="1">
+        <v>0</v>
+      </c>
+      <c r="J120" s="1">
+        <v>0</v>
+      </c>
+      <c r="K120" s="1">
+        <v>0</v>
+      </c>
+      <c r="L120" s="1">
+        <v>12</v>
+      </c>
+      <c r="M120" s="1">
+        <v>0</v>
+      </c>
+      <c r="N120" s="1">
+        <v>0</v>
+      </c>
+      <c r="O120" s="1">
+        <v>21</v>
+      </c>
+      <c r="P120" s="13">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q120" s="13">
+        <v>0</v>
+      </c>
+      <c r="R120" s="13">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="S120" s="1">
+        <v>0</v>
+      </c>
+      <c r="T120" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D121" s="1">
+        <v>0</v>
+      </c>
+      <c r="E121" s="1">
+        <v>1</v>
+      </c>
+      <c r="F121" s="1">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0</v>
+      </c>
+      <c r="H121" s="1">
+        <v>2</v>
+      </c>
+      <c r="I121" s="1">
+        <v>1</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0</v>
+      </c>
+      <c r="K121" s="1">
+        <v>0</v>
+      </c>
+      <c r="L121" s="1">
+        <v>2</v>
+      </c>
+      <c r="M121" s="1">
+        <v>1</v>
+      </c>
+      <c r="N121" s="1">
+        <v>0</v>
+      </c>
+      <c r="O121" s="1">
+        <v>19</v>
+      </c>
+      <c r="P121" s="13">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="Q121" s="13">
+        <v>0</v>
+      </c>
+      <c r="R121" s="13">
+        <v>0.53402777777777777</v>
+      </c>
+      <c r="S121" s="1">
+        <v>0</v>
+      </c>
+      <c r="T121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1</v>
+      </c>
+      <c r="E122" s="1">
+        <v>0</v>
+      </c>
+      <c r="F122" s="1">
+        <v>0</v>
+      </c>
+      <c r="G122" s="1">
+        <v>1</v>
+      </c>
+      <c r="H122" s="1">
+        <v>0</v>
+      </c>
+      <c r="I122" s="1">
+        <v>1</v>
+      </c>
+      <c r="J122" s="1">
+        <v>0</v>
+      </c>
+      <c r="K122" s="1">
+        <v>0</v>
+      </c>
+      <c r="L122" s="1">
+        <v>2</v>
+      </c>
+      <c r="M122" s="1">
+        <v>1</v>
+      </c>
+      <c r="N122" s="1">
+        <v>1</v>
+      </c>
+      <c r="O122" s="1">
+        <v>18</v>
+      </c>
+      <c r="P122" s="13">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="Q122" s="13">
+        <v>0</v>
+      </c>
+      <c r="R122" s="13">
+        <v>0.55069444444444449</v>
+      </c>
+      <c r="S122" s="1">
+        <v>0</v>
+      </c>
+      <c r="T122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D123" s="1">
+        <v>1</v>
+      </c>
+      <c r="E123" s="1">
+        <v>1</v>
+      </c>
+      <c r="F123" s="1">
+        <v>3</v>
+      </c>
+      <c r="G123" s="1">
+        <v>2</v>
+      </c>
+      <c r="H123" s="1">
+        <v>2</v>
+      </c>
+      <c r="I123" s="1">
+        <v>2</v>
+      </c>
+      <c r="J123" s="1">
+        <v>0</v>
+      </c>
+      <c r="K123" s="1">
+        <v>0</v>
+      </c>
+      <c r="L123" s="1">
+        <v>1</v>
+      </c>
+      <c r="M123" s="1">
+        <v>1</v>
+      </c>
+      <c r="N123" s="1">
+        <v>0</v>
+      </c>
+      <c r="O123" s="1">
+        <v>23</v>
+      </c>
+      <c r="P123" s="13">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="Q123" s="13">
+        <v>0</v>
+      </c>
+      <c r="R123" s="13">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="S123" s="1">
+        <v>1</v>
+      </c>
+      <c r="T123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D124" s="1">
+        <v>0</v>
+      </c>
+      <c r="E124" s="1">
+        <v>1</v>
+      </c>
+      <c r="F124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G124" s="1">
+        <v>3</v>
+      </c>
+      <c r="H124" s="1">
+        <v>3</v>
+      </c>
+      <c r="I124" s="1">
+        <v>2</v>
+      </c>
+      <c r="J124" s="1">
+        <v>0</v>
+      </c>
+      <c r="K124" s="1">
+        <v>0</v>
+      </c>
+      <c r="L124" s="1">
+        <v>2</v>
+      </c>
+      <c r="M124" s="1">
+        <v>0</v>
+      </c>
+      <c r="N124" s="1">
+        <v>0</v>
+      </c>
+      <c r="O124" s="1">
+        <v>22</v>
+      </c>
+      <c r="P124" s="13">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="Q124" s="13">
+        <v>0</v>
+      </c>
+      <c r="R124" s="13">
+        <v>0.68611111111111101</v>
+      </c>
+      <c r="S124" s="1">
+        <v>8</v>
+      </c>
+      <c r="T124" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G125" s="1">
+        <v>0</v>
+      </c>
+      <c r="H125" s="1">
+        <v>0</v>
+      </c>
+      <c r="I125" s="1">
+        <v>4</v>
+      </c>
+      <c r="J125" s="1">
+        <v>0</v>
+      </c>
+      <c r="K125" s="1">
+        <v>0</v>
+      </c>
+      <c r="L125" s="1">
+        <v>6</v>
+      </c>
+      <c r="M125" s="1">
+        <v>0</v>
+      </c>
+      <c r="N125" s="1">
+        <v>0</v>
+      </c>
+      <c r="O125" s="1">
+        <v>14</v>
+      </c>
+      <c r="P125" s="13">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q125" s="13">
+        <v>0</v>
+      </c>
+      <c r="R125" s="13">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="S125" s="1">
+        <v>0</v>
+      </c>
+      <c r="T125" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0</v>
+      </c>
+      <c r="F126" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G126" s="1">
+        <v>0</v>
+      </c>
+      <c r="H126" s="1">
+        <v>0</v>
+      </c>
+      <c r="I126" s="1">
+        <v>1</v>
+      </c>
+      <c r="J126" s="1">
+        <v>0</v>
+      </c>
+      <c r="K126" s="1">
+        <v>0</v>
+      </c>
+      <c r="L126" s="1">
+        <v>0</v>
+      </c>
+      <c r="M126" s="1">
+        <v>1</v>
+      </c>
+      <c r="N126" s="1">
+        <v>1</v>
+      </c>
+      <c r="O126" s="1">
+        <v>14</v>
+      </c>
+      <c r="P126" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="13">
+        <v>0</v>
+      </c>
+      <c r="R126" s="13">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="S126" s="1">
+        <v>0</v>
+      </c>
+      <c r="T126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D127" s="1">
+        <v>0</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0</v>
+      </c>
+      <c r="F127" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G127" s="1">
+        <v>0</v>
+      </c>
+      <c r="H127" s="1">
+        <v>0</v>
+      </c>
+      <c r="I127" s="1">
+        <v>0</v>
+      </c>
+      <c r="J127" s="1">
+        <v>0</v>
+      </c>
+      <c r="K127" s="1">
+        <v>0</v>
+      </c>
+      <c r="L127" s="1">
+        <v>0</v>
+      </c>
+      <c r="M127" s="1">
+        <v>0</v>
+      </c>
+      <c r="N127" s="1">
+        <v>2</v>
+      </c>
+      <c r="O127" s="1">
+        <v>15</v>
+      </c>
+      <c r="P127" s="13">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="Q127" s="13">
+        <v>0</v>
+      </c>
+      <c r="R127" s="13">
+        <v>0.48472222222222222</v>
+      </c>
+      <c r="S127" s="1">
+        <v>0</v>
+      </c>
+      <c r="T127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" s="1">
+        <v>0</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1</v>
+      </c>
+      <c r="F128" s="1">
+        <v>1</v>
+      </c>
+      <c r="G128" s="1">
+        <v>1</v>
+      </c>
+      <c r="H128" s="1">
+        <v>0</v>
+      </c>
+      <c r="I128" s="1">
+        <v>3</v>
+      </c>
+      <c r="J128" s="1">
+        <v>0</v>
+      </c>
+      <c r="K128" s="1">
+        <v>0</v>
+      </c>
+      <c r="L128" s="1">
+        <v>2</v>
+      </c>
+      <c r="M128" s="1">
+        <v>0</v>
+      </c>
+      <c r="N128" s="1">
+        <v>1</v>
+      </c>
+      <c r="O128" s="1">
+        <v>25</v>
+      </c>
+      <c r="P128" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="13">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="R128" s="13">
+        <v>0.88750000000000007</v>
+      </c>
+      <c r="S128" s="1">
+        <v>0</v>
+      </c>
+      <c r="T128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="1">
+        <v>0</v>
+      </c>
+      <c r="E129" s="1">
+        <v>1</v>
+      </c>
+      <c r="F129" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G129" s="1">
+        <v>3</v>
+      </c>
+      <c r="H129" s="1">
+        <v>2</v>
+      </c>
+      <c r="I129" s="1">
+        <v>0</v>
+      </c>
+      <c r="J129" s="1">
+        <v>0</v>
+      </c>
+      <c r="K129" s="1">
+        <v>0</v>
+      </c>
+      <c r="L129" s="1">
+        <v>1</v>
+      </c>
+      <c r="M129" s="1">
+        <v>0</v>
+      </c>
+      <c r="N129" s="1">
+        <v>0</v>
+      </c>
+      <c r="O129" s="1">
+        <v>18</v>
+      </c>
+      <c r="P129" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="13">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="R129" s="13">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="S129" s="1">
+        <v>1</v>
+      </c>
+      <c r="T129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0</v>
+      </c>
+      <c r="E130" s="1">
+        <v>0</v>
+      </c>
+      <c r="F130" s="1">
+        <v>-4</v>
+      </c>
+      <c r="G130" s="1">
+        <v>3</v>
+      </c>
+      <c r="H130" s="1">
+        <v>0</v>
+      </c>
+      <c r="I130" s="1">
+        <v>1</v>
+      </c>
+      <c r="J130" s="1">
+        <v>1</v>
+      </c>
+      <c r="K130" s="1">
+        <v>2</v>
+      </c>
+      <c r="L130" s="1">
+        <v>1</v>
+      </c>
+      <c r="M130" s="1">
+        <v>0</v>
+      </c>
+      <c r="N130" s="1">
+        <v>2</v>
+      </c>
+      <c r="O130" s="1">
+        <v>24</v>
+      </c>
+      <c r="P130" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="13">
+        <v>0</v>
+      </c>
+      <c r="R130" s="13">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="S130" s="1">
+        <v>0</v>
+      </c>
+      <c r="T130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" s="1">
+        <v>0</v>
+      </c>
+      <c r="E131" s="1">
+        <v>0</v>
+      </c>
+      <c r="F131" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G131" s="1">
+        <v>0</v>
+      </c>
+      <c r="H131" s="1">
+        <v>1</v>
+      </c>
+      <c r="I131" s="1">
+        <v>0</v>
+      </c>
+      <c r="J131" s="1">
+        <v>0</v>
+      </c>
+      <c r="K131" s="1">
+        <v>0</v>
+      </c>
+      <c r="L131" s="1">
+        <v>3</v>
+      </c>
+      <c r="M131" s="1">
+        <v>0</v>
+      </c>
+      <c r="N131" s="1">
+        <v>1</v>
+      </c>
+      <c r="O131" s="1">
+        <v>17</v>
+      </c>
+      <c r="P131" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="13">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="R131" s="13">
+        <v>0.5229166666666667</v>
+      </c>
+      <c r="S131" s="1">
+        <v>1</v>
+      </c>
+      <c r="T131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D132" s="1">
+        <v>0</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0</v>
+      </c>
+      <c r="F132" s="1">
+        <v>0</v>
+      </c>
+      <c r="G132" s="1">
+        <v>3</v>
+      </c>
+      <c r="H132" s="1">
+        <v>0</v>
+      </c>
+      <c r="I132" s="1">
+        <v>0</v>
+      </c>
+      <c r="J132" s="1">
+        <v>0</v>
+      </c>
+      <c r="K132" s="1">
+        <v>0</v>
+      </c>
+      <c r="L132" s="1">
+        <v>4</v>
+      </c>
+      <c r="M132" s="1">
+        <v>0</v>
+      </c>
+      <c r="N132" s="1">
+        <v>0</v>
+      </c>
+      <c r="O132" s="1">
+        <v>18</v>
+      </c>
+      <c r="P132" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q132" s="13">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="R132" s="13">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="S132" s="1">
+        <v>1</v>
+      </c>
+      <c r="T132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D133" s="1">
+        <v>0</v>
+      </c>
+      <c r="E133" s="1">
+        <v>0</v>
+      </c>
+      <c r="F133" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G133" s="1">
+        <v>0</v>
+      </c>
+      <c r="H133" s="1">
+        <v>1</v>
+      </c>
+      <c r="I133" s="1">
+        <v>0</v>
+      </c>
+      <c r="J133" s="1">
+        <v>0</v>
+      </c>
+      <c r="K133" s="1">
+        <v>0</v>
+      </c>
+      <c r="L133" s="1">
+        <v>2</v>
+      </c>
+      <c r="M133" s="1">
+        <v>1</v>
+      </c>
+      <c r="N133" s="1">
+        <v>1</v>
+      </c>
+      <c r="O133" s="1">
+        <v>22</v>
+      </c>
+      <c r="P133" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q133" s="13">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="R133" s="13">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="S133" s="1">
+        <v>7</v>
+      </c>
+      <c r="T133" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0</v>
+      </c>
+      <c r="F134" s="1">
+        <v>0</v>
+      </c>
+      <c r="G134" s="1">
+        <v>1</v>
+      </c>
+      <c r="H134" s="1">
+        <v>4</v>
+      </c>
+      <c r="I134" s="1">
+        <v>0</v>
+      </c>
+      <c r="J134" s="1">
+        <v>0</v>
+      </c>
+      <c r="K134" s="1">
+        <v>0</v>
+      </c>
+      <c r="L134" s="1">
+        <v>4</v>
+      </c>
+      <c r="M134" s="1">
+        <v>0</v>
+      </c>
+      <c r="N134" s="1">
+        <v>0</v>
+      </c>
+      <c r="O134" s="1">
+        <v>15</v>
+      </c>
+      <c r="P134" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="13">
+        <v>0</v>
+      </c>
+      <c r="R134" s="13">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="S134" s="1">
+        <v>0</v>
+      </c>
+      <c r="T134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" s="1">
+        <v>0</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0</v>
+      </c>
+      <c r="F135" s="1">
+        <v>-3</v>
+      </c>
+      <c r="G135" s="1">
+        <v>1</v>
+      </c>
+      <c r="H135" s="1">
+        <v>0</v>
+      </c>
+      <c r="I135" s="1">
+        <v>1</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0</v>
+      </c>
+      <c r="K135" s="1">
+        <v>0</v>
+      </c>
+      <c r="L135" s="1">
+        <v>3</v>
+      </c>
+      <c r="M135" s="1">
+        <v>1</v>
+      </c>
+      <c r="N135" s="1">
+        <v>0</v>
+      </c>
+      <c r="O135" s="1">
+        <v>20</v>
+      </c>
+      <c r="P135" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="13">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="R135" s="13">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="S135" s="1">
+        <v>0</v>
+      </c>
+      <c r="T135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D136" s="1">
+        <v>0</v>
+      </c>
+      <c r="E136" s="1">
+        <v>0</v>
+      </c>
+      <c r="F136" s="1">
+        <v>1</v>
+      </c>
+      <c r="G136" s="1">
+        <v>2</v>
+      </c>
+      <c r="H136" s="1">
+        <v>3</v>
+      </c>
+      <c r="I136" s="1">
+        <v>3</v>
+      </c>
+      <c r="J136" s="1">
+        <v>0</v>
+      </c>
+      <c r="K136" s="1">
+        <v>0</v>
+      </c>
+      <c r="L136" s="1">
+        <v>3</v>
+      </c>
+      <c r="M136" s="1">
+        <v>0</v>
+      </c>
+      <c r="N136" s="1">
+        <v>3</v>
+      </c>
+      <c r="O136" s="1">
+        <v>24</v>
+      </c>
+      <c r="P136" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q136" s="13">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="R136" s="13">
+        <v>0.78125</v>
+      </c>
+      <c r="S136" s="1">
+        <v>0</v>
+      </c>
+      <c r="T136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0</v>
+      </c>
+      <c r="E137" s="1">
+        <v>0</v>
+      </c>
+      <c r="F137" s="1">
+        <v>0</v>
+      </c>
+      <c r="G137" s="1">
+        <v>0</v>
+      </c>
+      <c r="H137" s="1">
+        <v>2</v>
+      </c>
+      <c r="I137" s="1">
+        <v>0</v>
+      </c>
+      <c r="J137" s="1">
+        <v>0</v>
+      </c>
+      <c r="K137" s="1">
+        <v>0</v>
+      </c>
+      <c r="L137" s="1">
+        <v>0</v>
+      </c>
+      <c r="M137" s="1">
+        <v>0</v>
+      </c>
+      <c r="N137" s="1">
+        <v>1</v>
+      </c>
+      <c r="O137" s="1">
+        <v>14</v>
+      </c>
+      <c r="P137" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="13">
+        <v>0</v>
+      </c>
+      <c r="R137" s="13">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="S137" s="1">
+        <v>2</v>
+      </c>
+      <c r="T137" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="1">
+        <v>1</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1</v>
+      </c>
+      <c r="G138" s="1">
+        <v>5</v>
+      </c>
+      <c r="H138" s="1">
+        <v>3</v>
+      </c>
+      <c r="I138" s="1">
+        <v>2</v>
+      </c>
+      <c r="J138" s="1">
+        <v>0</v>
+      </c>
+      <c r="K138" s="1">
+        <v>0</v>
+      </c>
+      <c r="L138" s="1">
+        <v>3</v>
+      </c>
+      <c r="M138" s="1">
+        <v>1</v>
+      </c>
+      <c r="N138" s="1">
+        <v>2</v>
+      </c>
+      <c r="O138" s="1">
+        <v>27</v>
+      </c>
+      <c r="P138" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="13">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="R138" s="13">
+        <v>0.93541666666666667</v>
+      </c>
+      <c r="S138" s="1">
+        <v>0</v>
+      </c>
+      <c r="T138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" s="1">
+        <v>0</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0</v>
+      </c>
+      <c r="F139" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G139" s="1">
+        <v>5</v>
+      </c>
+      <c r="H139" s="1">
+        <v>3</v>
+      </c>
+      <c r="I139" s="1">
+        <v>0</v>
+      </c>
+      <c r="J139" s="1">
+        <v>0</v>
+      </c>
+      <c r="K139" s="1">
+        <v>0</v>
+      </c>
+      <c r="L139" s="1">
+        <v>1</v>
+      </c>
+      <c r="M139" s="1">
+        <v>1</v>
+      </c>
+      <c r="N139" s="1">
+        <v>0</v>
+      </c>
+      <c r="O139" s="1">
+        <v>18</v>
+      </c>
+      <c r="P139" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="13">
+        <v>0</v>
+      </c>
+      <c r="R139" s="13">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="S139" s="1">
+        <v>0</v>
+      </c>
+      <c r="T139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140" s="1">
+        <v>0</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0</v>
+      </c>
+      <c r="F140" s="1">
+        <v>1</v>
+      </c>
+      <c r="G140" s="1">
+        <v>1</v>
+      </c>
+      <c r="H140" s="1">
+        <v>1</v>
+      </c>
+      <c r="I140" s="1">
+        <v>0</v>
+      </c>
+      <c r="J140" s="1">
+        <v>0</v>
+      </c>
+      <c r="K140" s="1">
+        <v>0</v>
+      </c>
+      <c r="L140" s="1">
+        <v>0</v>
+      </c>
+      <c r="M140" s="1">
+        <v>0</v>
+      </c>
+      <c r="N140" s="1">
+        <v>0</v>
+      </c>
+      <c r="O140" s="1">
+        <v>20</v>
+      </c>
+      <c r="P140" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="13">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="R140" s="13">
+        <v>0.62430555555555556</v>
+      </c>
+      <c r="S140" s="1">
+        <v>0</v>
+      </c>
+      <c r="T140" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D141" s="1">
+        <v>0</v>
+      </c>
+      <c r="E141" s="1">
+        <v>0</v>
+      </c>
+      <c r="F141" s="1">
+        <v>-4</v>
+      </c>
+      <c r="G141" s="1">
+        <v>0</v>
+      </c>
+      <c r="H141" s="1">
+        <v>0</v>
+      </c>
+      <c r="I141" s="1">
+        <v>1</v>
+      </c>
+      <c r="J141" s="1">
+        <v>0</v>
+      </c>
+      <c r="K141" s="1">
+        <v>0</v>
+      </c>
+      <c r="L141" s="1">
+        <v>0</v>
+      </c>
+      <c r="M141" s="1">
+        <v>1</v>
+      </c>
+      <c r="N141" s="1">
+        <v>2</v>
+      </c>
+      <c r="O141" s="1">
+        <v>22</v>
+      </c>
+      <c r="P141" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q141" s="13">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="R141" s="13">
+        <v>0.70208333333333339</v>
+      </c>
+      <c r="S141" s="1">
+        <v>0</v>
+      </c>
+      <c r="T141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="1">
+        <v>1</v>
+      </c>
+      <c r="E142" s="1">
+        <v>0</v>
+      </c>
+      <c r="F142" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G142" s="1">
+        <v>3</v>
+      </c>
+      <c r="H142" s="1">
+        <v>0</v>
+      </c>
+      <c r="I142" s="1">
+        <v>0</v>
+      </c>
+      <c r="J142" s="1">
+        <v>0</v>
+      </c>
+      <c r="K142" s="1">
+        <v>0</v>
+      </c>
+      <c r="L142" s="1">
+        <v>1</v>
+      </c>
+      <c r="M142" s="1">
+        <v>0</v>
+      </c>
+      <c r="N142" s="1">
+        <v>0</v>
+      </c>
+      <c r="O142" s="1">
+        <v>18</v>
+      </c>
+      <c r="P142" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q142" s="13">
+        <v>0</v>
+      </c>
+      <c r="R142" s="13">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="S142" s="1">
+        <v>14</v>
+      </c>
+      <c r="T142" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="1">
+        <v>0</v>
+      </c>
+      <c r="E143" s="1">
+        <v>0</v>
+      </c>
+      <c r="F143" s="1">
+        <v>0</v>
+      </c>
+      <c r="G143" s="1">
+        <v>2</v>
+      </c>
+      <c r="H143" s="1">
+        <v>1</v>
+      </c>
+      <c r="I143" s="1">
+        <v>0</v>
+      </c>
+      <c r="J143" s="1">
+        <v>0</v>
+      </c>
+      <c r="K143" s="1">
+        <v>0</v>
+      </c>
+      <c r="L143" s="1">
+        <v>1</v>
+      </c>
+      <c r="M143" s="1">
+        <v>0</v>
+      </c>
+      <c r="N143" s="1">
+        <v>0</v>
+      </c>
+      <c r="O143" s="1">
+        <v>19</v>
+      </c>
+      <c r="P143" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q143" s="13">
+        <v>0</v>
+      </c>
+      <c r="R143" s="13">
+        <v>0.61249999999999993</v>
+      </c>
+      <c r="S143" s="1">
+        <v>0</v>
+      </c>
+      <c r="T143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="1">
+        <v>0</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0</v>
+      </c>
+      <c r="F144" s="1">
+        <v>0</v>
+      </c>
+      <c r="G144" s="1">
+        <v>1</v>
+      </c>
+      <c r="H144" s="1">
+        <v>1</v>
+      </c>
+      <c r="I144" s="1">
+        <v>0</v>
+      </c>
+      <c r="J144" s="1">
+        <v>0</v>
+      </c>
+      <c r="K144" s="1">
+        <v>0</v>
+      </c>
+      <c r="L144" s="1">
+        <v>0</v>
+      </c>
+      <c r="M144" s="1">
+        <v>1</v>
+      </c>
+      <c r="N144" s="1">
+        <v>1</v>
+      </c>
+      <c r="O144" s="1">
+        <v>20</v>
+      </c>
+      <c r="P144" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q144" s="13">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="R144" s="13">
+        <v>0.6020833333333333</v>
+      </c>
+      <c r="S144" s="1">
+        <v>4</v>
+      </c>
+      <c r="T144" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0</v>
+      </c>
+      <c r="F145" s="1">
+        <v>0</v>
+      </c>
+      <c r="G145" s="1">
+        <v>1</v>
+      </c>
+      <c r="H145" s="1">
+        <v>1</v>
+      </c>
+      <c r="I145" s="1">
+        <v>2</v>
+      </c>
+      <c r="J145" s="1">
+        <v>0</v>
+      </c>
+      <c r="K145" s="1">
+        <v>0</v>
+      </c>
+      <c r="L145" s="1">
+        <v>1</v>
+      </c>
+      <c r="M145" s="1">
+        <v>0</v>
+      </c>
+      <c r="N145" s="1">
+        <v>1</v>
+      </c>
+      <c r="O145" s="1">
+        <v>22</v>
+      </c>
+      <c r="P145" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q145" s="13">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="R145" s="13">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="S145" s="1">
+        <v>0</v>
+      </c>
+      <c r="T145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P146" s="1"/>
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P147" s="1"/>
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P148" s="1"/>
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P149" s="1"/>
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P150" s="1"/>
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P151" s="1"/>
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P152" s="1"/>
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P153" s="1"/>
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P154" s="1"/>
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P155" s="1"/>
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P156" s="1"/>
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P157" s="1"/>
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P158" s="1"/>
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P159" s="1"/>
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P160" s="1"/>
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
@@ -31505,220 +33554,144 @@
       <c r="R193" s="1"/>
     </row>
     <row r="194" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P194" s="1"/>
-      <c r="Q194" s="1"/>
       <c r="R194" s="1"/>
     </row>
     <row r="195" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P195" s="1"/>
-      <c r="Q195" s="1"/>
       <c r="R195" s="1"/>
     </row>
     <row r="196" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P196" s="1"/>
-      <c r="Q196" s="1"/>
       <c r="R196" s="1"/>
     </row>
     <row r="197" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P197" s="1"/>
-      <c r="Q197" s="1"/>
       <c r="R197" s="1"/>
     </row>
     <row r="198" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P198" s="1"/>
-      <c r="Q198" s="1"/>
       <c r="R198" s="1"/>
     </row>
     <row r="199" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P199" s="1"/>
-      <c r="Q199" s="1"/>
       <c r="R199" s="1"/>
     </row>
     <row r="200" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P200" s="1"/>
-      <c r="Q200" s="1"/>
       <c r="R200" s="1"/>
     </row>
     <row r="201" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P201" s="1"/>
-      <c r="Q201" s="1"/>
       <c r="R201" s="1"/>
     </row>
     <row r="202" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P202" s="1"/>
-      <c r="Q202" s="1"/>
       <c r="R202" s="1"/>
     </row>
     <row r="203" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P203" s="1"/>
-      <c r="Q203" s="1"/>
       <c r="R203" s="1"/>
     </row>
     <row r="204" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P204" s="1"/>
-      <c r="Q204" s="1"/>
       <c r="R204" s="1"/>
     </row>
     <row r="205" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P205" s="1"/>
-      <c r="Q205" s="1"/>
       <c r="R205" s="1"/>
     </row>
     <row r="206" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P206" s="1"/>
-      <c r="Q206" s="1"/>
       <c r="R206" s="1"/>
     </row>
     <row r="207" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P207" s="1"/>
-      <c r="Q207" s="1"/>
       <c r="R207" s="1"/>
     </row>
     <row r="208" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P208" s="1"/>
-      <c r="Q208" s="1"/>
       <c r="R208" s="1"/>
     </row>
-    <row r="209" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P209" s="1"/>
-      <c r="Q209" s="1"/>
+    <row r="209" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R209" s="1"/>
     </row>
-    <row r="210" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P210" s="1"/>
-      <c r="Q210" s="1"/>
+    <row r="210" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R210" s="1"/>
     </row>
-    <row r="211" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P211" s="1"/>
-      <c r="Q211" s="1"/>
+    <row r="211" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R211" s="1"/>
     </row>
-    <row r="212" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P212" s="1"/>
-      <c r="Q212" s="1"/>
+    <row r="212" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R212" s="1"/>
     </row>
-    <row r="213" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P213" s="1"/>
-      <c r="Q213" s="1"/>
+    <row r="213" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R213" s="1"/>
     </row>
-    <row r="214" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P214" s="1"/>
-      <c r="Q214" s="1"/>
+    <row r="214" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R214" s="1"/>
     </row>
-    <row r="215" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P215" s="1"/>
-      <c r="Q215" s="1"/>
+    <row r="215" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R215" s="1"/>
     </row>
-    <row r="216" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P216" s="1"/>
-      <c r="Q216" s="1"/>
+    <row r="216" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R216" s="1"/>
     </row>
-    <row r="217" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P217" s="1"/>
-      <c r="Q217" s="1"/>
+    <row r="217" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R217" s="1"/>
     </row>
-    <row r="218" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P218" s="1"/>
-      <c r="Q218" s="1"/>
+    <row r="218" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R218" s="1"/>
     </row>
-    <row r="219" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P219" s="1"/>
-      <c r="Q219" s="1"/>
+    <row r="219" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R219" s="1"/>
     </row>
-    <row r="220" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P220" s="1"/>
-      <c r="Q220" s="1"/>
+    <row r="220" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R220" s="1"/>
     </row>
-    <row r="221" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P221" s="1"/>
-      <c r="Q221" s="1"/>
+    <row r="221" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R221" s="1"/>
     </row>
-    <row r="222" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P222" s="1"/>
-      <c r="Q222" s="1"/>
+    <row r="222" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R222" s="1"/>
     </row>
-    <row r="223" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P223" s="1"/>
-      <c r="Q223" s="1"/>
+    <row r="223" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R223" s="1"/>
     </row>
-    <row r="224" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P224" s="1"/>
-      <c r="Q224" s="1"/>
+    <row r="224" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R224" s="1"/>
     </row>
-    <row r="225" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P225" s="1"/>
-      <c r="Q225" s="1"/>
+    <row r="225" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R225" s="1"/>
     </row>
-    <row r="226" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P226" s="1"/>
-      <c r="Q226" s="1"/>
+    <row r="226" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R226" s="1"/>
     </row>
-    <row r="227" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P227" s="1"/>
-      <c r="Q227" s="1"/>
+    <row r="227" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R227" s="1"/>
     </row>
-    <row r="228" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P228" s="1"/>
-      <c r="Q228" s="1"/>
+    <row r="228" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R228" s="1"/>
     </row>
-    <row r="229" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P229" s="1"/>
-      <c r="Q229" s="1"/>
+    <row r="229" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R229" s="1"/>
     </row>
-    <row r="230" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P230" s="1"/>
-      <c r="Q230" s="1"/>
+    <row r="230" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R230" s="1"/>
     </row>
-    <row r="231" spans="16:18" x14ac:dyDescent="0.25">
-      <c r="P231" s="1"/>
-      <c r="Q231" s="1"/>
+    <row r="231" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R231" s="1"/>
     </row>
-    <row r="232" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="232" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R232" s="1"/>
     </row>
-    <row r="233" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="233" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R233" s="1"/>
     </row>
-    <row r="234" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="234" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R234" s="1"/>
     </row>
-    <row r="235" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="235" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R235" s="1"/>
     </row>
-    <row r="236" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="236" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R236" s="1"/>
     </row>
-    <row r="237" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="237" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R237" s="1"/>
     </row>
-    <row r="238" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="238" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R238" s="1"/>
     </row>
-    <row r="239" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="239" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R239" s="1"/>
     </row>
-    <row r="240" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="240" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R240" s="1"/>
     </row>
     <row r="241" spans="18:18" x14ac:dyDescent="0.25">
@@ -31745,127 +33718,12 @@
     <row r="248" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R248" s="1"/>
     </row>
-    <row r="249" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R249" s="1"/>
-    </row>
-    <row r="250" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R250" s="1"/>
-    </row>
-    <row r="251" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R251" s="1"/>
-    </row>
-    <row r="252" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R252" s="1"/>
-    </row>
-    <row r="253" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R253" s="1"/>
-    </row>
-    <row r="254" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R254" s="1"/>
-    </row>
-    <row r="255" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R255" s="1"/>
-    </row>
-    <row r="256" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R256" s="1"/>
-    </row>
-    <row r="257" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R257" s="1"/>
-    </row>
-    <row r="258" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R258" s="1"/>
-    </row>
-    <row r="259" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R259" s="1"/>
-    </row>
-    <row r="260" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R260" s="1"/>
-    </row>
-    <row r="261" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R261" s="1"/>
-    </row>
-    <row r="262" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R262" s="1"/>
-    </row>
-    <row r="263" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R263" s="1"/>
-    </row>
-    <row r="264" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R264" s="1"/>
-    </row>
-    <row r="265" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R265" s="1"/>
-    </row>
-    <row r="266" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R266" s="1"/>
-    </row>
-    <row r="267" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R267" s="1"/>
-    </row>
-    <row r="268" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R268" s="1"/>
-    </row>
-    <row r="269" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R269" s="1"/>
-    </row>
-    <row r="270" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R270" s="1"/>
-    </row>
-    <row r="271" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R271" s="1"/>
-    </row>
-    <row r="272" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R272" s="1"/>
-    </row>
-    <row r="273" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R273" s="1"/>
-    </row>
-    <row r="274" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R274" s="1"/>
-    </row>
-    <row r="275" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R275" s="1"/>
-    </row>
-    <row r="276" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R276" s="1"/>
-    </row>
-    <row r="277" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R277" s="1"/>
-    </row>
-    <row r="278" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R278" s="1"/>
-    </row>
-    <row r="279" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R279" s="1"/>
-    </row>
-    <row r="280" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R280" s="1"/>
-    </row>
-    <row r="281" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R281" s="1"/>
-    </row>
-    <row r="282" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R282" s="1"/>
-    </row>
-    <row r="283" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R283" s="1"/>
-    </row>
-    <row r="284" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R284" s="1"/>
-    </row>
-    <row r="285" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R285" s="1"/>
-    </row>
-    <row r="286" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R286" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T286">
-    <sortCondition ref="C2:C286"/>
-    <sortCondition ref="A2:A286"/>
+  <sortState ref="A111:V128">
+    <sortCondition ref="A111"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-22-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-22-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -31873,7 +33731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -32101,7 +33959,7 @@
       <c r="M55" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C17">
+  <sortState ref="C2:C17">
     <sortCondition ref="C2:C17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32109,7 +33967,467 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="14">
+        <v>2.4902777777777776</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>2.6312500000000001</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="14">
+        <v>2.6312500000000001</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="14">
+        <v>2.4812500000000002</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="14">
+        <v>2.46875</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="14">
+        <v>2.442361111111111</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M1" location="'Scores (4-22-25)'!A1" display="HOME"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1"/>
+    <col min="4" max="15" width="9.140625" style="1"/>
+    <col min="16" max="18" width="9.140625" style="13"/>
+    <col min="19" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U1" location="'Scores (4-23-25)'!A1" display="HOME"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34930,8 +37248,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34988,248 +37306,38 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="14">
-        <v>2.4902777777777776</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="14">
-        <v>2.5</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14">
-        <v>2.6312500000000001</v>
-      </c>
-      <c r="L4" s="1">
-        <v>2</v>
-      </c>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-      <c r="K5" s="14">
-        <v>2.6312500000000001</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14">
-        <v>2.4812500000000002</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="14">
-        <v>2.46875</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
+      <c r="K7" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-22-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-23-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35710,182 +37818,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="15" width="9.140625" style="1"/>
-    <col min="16" max="18" width="9.140625" style="13"/>
-    <col min="19" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-23-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:M7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K3" s="14"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K4" s="14"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K7" s="14"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-23-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35971,7 +37905,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-24-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-24-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -35979,7 +37913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36055,7 +37989,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-24-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-24-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36063,7 +37997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36147,7 +38081,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-25-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-25-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36155,7 +38089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36229,7 +38163,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-25-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-25-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36237,7 +38171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36321,7 +38255,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-26-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-26-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36329,7 +38263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36419,21 +38353,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="A5" location="'Offense (4-19-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="A6" location="'Goalies (4-19-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A5" location="'Offense (4-19-25)'!A1" display="Offense"/>
+    <hyperlink ref="A6" location="'Goalies (4-19-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -36446,7 +38380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36520,7 +38454,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-26-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-26-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36528,7 +38462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36614,7 +38548,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-27-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="U1" location="'Scores (4-27-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36622,7 +38556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36698,7 +38632,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-27-25)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="M1" location="'Scores (4-27-25)'!A1" display="HOME"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -36706,7 +38640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36810,21 +38744,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="A6" location="'Offense (4-20-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="A7" location="'Goalies (4-20-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A6" location="'Offense (4-20-25)'!A1" display="Offense"/>
+    <hyperlink ref="A7" location="'Goalies (4-20-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -36837,7 +38771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36961,21 +38895,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="A7" location="'Offense (4-21-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="A8" location="'Goalies (4-21-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A7" location="'Offense (4-21-25)'!A1" display="Offense"/>
+    <hyperlink ref="A8" location="'Goalies (4-21-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -36988,11 +38922,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37084,11 +39018,15 @@
       <c r="A6" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
       <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -37105,21 +39043,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="A7" location="'Offense (4-22-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="A8" location="'Goalies (4-22-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A7" location="'Offense (4-22-25)'!A1" display="Offense"/>
+    <hyperlink ref="A8" location="'Goalies (4-22-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -37132,10 +39070,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -37224,21 +39162,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="A6" location="'Offense (4-23-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="A7" location="'Goalies (4-23-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A6" location="'Offense (4-23-25)'!A1" display="Offense"/>
+    <hyperlink ref="A7" location="'Goalies (4-23-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -37251,7 +39189,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37353,21 +39291,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="A7" location="'Offense (4-24-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="A8" location="'Goalies (4-24-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A7" location="'Offense (4-24-25)'!A1" display="Offense"/>
+    <hyperlink ref="A8" location="'Goalies (4-24-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -37380,7 +39318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37472,21 +39410,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="A6" location="'Offense (4-25-25)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="A7" location="'Goalies (4-25-25)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
+    <hyperlink ref="A6" location="'Offense (4-25-25)'!A1" display="Offense"/>
+    <hyperlink ref="A7" location="'Goalies (4-25-25)'!A1" display="Goalies"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>

</xml_diff>